<commit_message>
fix excel date col
</commit_message>
<xml_diff>
--- a/TableS1_datasources.xlsx
+++ b/TableS1_datasources.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qread\google_drive\SESYNC Food Waste\MS4_VirtualLand\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qread\Documents\GitHub\foodwaste\virtualland\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="140">
   <si>
     <t>Dataset name</t>
   </si>
@@ -300,9 +300,6 @@
   </si>
   <si>
     <t>Olson, D. M. and E. Dinerstein. 2002. The Global 200: Priority ecoregions for global conservation. (PDF file) Annals of the Missouri Botanical Garden 89:125-126.</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>United States county boundaries shapefile</t>
@@ -789,7 +786,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +802,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -834,7 +831,7 @@
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -858,12 +855,12 @@
         <v>44278</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -892,7 +889,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -921,7 +918,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -950,7 +947,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -965,7 +962,7 @@
         <v>43</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G6" s="2">
         <v>44306</v>
@@ -974,12 +971,12 @@
         <v>44306</v>
       </c>
       <c r="I6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -1008,7 +1005,7 @@
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -1037,7 +1034,7 @@
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
@@ -1066,7 +1063,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
@@ -1095,7 +1092,7 @@
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
@@ -1124,7 +1121,7 @@
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -1153,7 +1150,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
         <v>87</v>
@@ -1182,10 +1179,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -1194,39 +1191,36 @@
         <v>2014</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" t="s">
         <v>94</v>
-      </c>
-      <c r="F14" t="s">
-        <v>95</v>
       </c>
       <c r="G14" s="2">
         <v>43069</v>
       </c>
-      <c r="H14" t="s">
-        <v>92</v>
-      </c>
       <c r="I14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" t="s">
         <v>97</v>
-      </c>
-      <c r="C15" t="s">
-        <v>98</v>
       </c>
       <c r="D15">
         <v>2020</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" t="s">
         <v>99</v>
-      </c>
-      <c r="F15" t="s">
-        <v>100</v>
       </c>
       <c r="G15" s="2">
         <v>44090</v>
@@ -1235,27 +1229,27 @@
         <v>44284</v>
       </c>
       <c r="I15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" t="s">
         <v>102</v>
-      </c>
-      <c r="C16" t="s">
-        <v>103</v>
       </c>
       <c r="D16">
         <v>2016</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" t="s">
         <v>104</v>
-      </c>
-      <c r="F16" t="s">
-        <v>105</v>
       </c>
       <c r="G16" s="2">
         <v>43724</v>
@@ -1264,27 +1258,27 @@
         <v>44284</v>
       </c>
       <c r="I16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17">
         <v>2016</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" t="s">
         <v>108</v>
-      </c>
-      <c r="F17" t="s">
-        <v>109</v>
       </c>
       <c r="G17" s="2">
         <v>44231</v>
@@ -1293,27 +1287,27 @@
         <v>44284</v>
       </c>
       <c r="I17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D18">
         <v>2001</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" t="s">
         <v>111</v>
-      </c>
-      <c r="F18" t="s">
-        <v>112</v>
       </c>
       <c r="G18" s="2">
         <v>44231</v>
@@ -1322,27 +1316,27 @@
         <v>44284</v>
       </c>
       <c r="I18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" t="s">
         <v>114</v>
-      </c>
-      <c r="C19" t="s">
-        <v>115</v>
       </c>
       <c r="D19">
         <v>2000</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>117</v>
       </c>
       <c r="G19" s="2">
         <v>44090</v>
@@ -1351,27 +1345,27 @@
         <v>44284</v>
       </c>
       <c r="I19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D20">
         <v>2010</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G20" s="2">
         <v>44090</v>
@@ -1380,27 +1374,27 @@
         <v>44284</v>
       </c>
       <c r="I20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D21">
         <v>2010</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="G21" s="2">
         <v>44057</v>
@@ -1409,26 +1403,26 @@
         <v>44284</v>
       </c>
       <c r="I21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="C22" t="s">
-        <v>133</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
         <v>73</v>
@@ -1452,12 +1446,12 @@
         <v>44348</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
         <v>74</v>
@@ -1466,7 +1460,7 @@
         <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>75</v>
@@ -1481,12 +1475,12 @@
         <v>44348</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B25" t="s">
         <v>68</v>
@@ -1515,7 +1509,7 @@
     </row>
     <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
         <v>67</v>
@@ -1539,18 +1533,18 @@
         <v>44278</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s">
         <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>72</v>
@@ -1558,13 +1552,13 @@
     </row>
     <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B28" t="s">
         <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>84</v>
@@ -1572,13 +1566,13 @@
     </row>
     <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
         <v>64</v>
       </c>
       <c r="C29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>85</v>
@@ -1586,13 +1580,13 @@
     </row>
     <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B30" t="s">
         <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>76</v>
@@ -1600,13 +1594,13 @@
     </row>
     <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B31" t="s">
         <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>77</v>
@@ -1614,13 +1608,13 @@
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B32" t="s">
         <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>70</v>
@@ -1628,13 +1622,13 @@
     </row>
     <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
         <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>78</v>

</xml_diff>